<commit_message>
Dépôt fichier pour soutenance
</commit_message>
<xml_diff>
--- a/P5_Takforyan-John_Gaelle/P5_02_plantests.xlsx
+++ b/P5_Takforyan-John_Gaelle/P5_02_plantests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelletakforyan/Desktop/Openclassrooms/Projet-5/P5_Takforyan-John_Gaelle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F849ACA6-5DBD-EE40-914E-75E737B465B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E237D12C-640E-124C-B5C1-A9647A49F0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>getTeddyData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La valeur retournée pourrait ne pas être disponible </t>
   </si>
   <si>
     <t>25 à 31</t>
@@ -144,10 +141,6 @@
 Si cette fonction affiche le bon produit alors c'est bon.</t>
   </si>
   <si>
-    <t xml:space="preserve">La valeur retournée pourrait être erronée (un autre produit au lieu du produit choisit) ou l'affichage ne fonctionnerait pas
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Appeler la fonction avec la méthode localStorage.setItem .
 </t>
   </si>
@@ -183,10 +176,6 @@
     <t>La fonction doit retourner à la page index.html si le panier/localStorage est vide. Si non, la fonction doit nous diriger à la page de validation.html .</t>
   </si>
   <si>
-    <t>La fonction doit ajouter le produit choisi et les inputs à l'intérieur du tableau.array.
-Ensuite il doit envoyer les données à la page suivante avec la méthode POST. La fonction doit retourner le local storage depuis le paramètre.</t>
-  </si>
-  <si>
     <t>La fonction doit retourner l'URL du produit séléctionné avec le nom de la peluche.</t>
   </si>
   <si>
@@ -205,22 +194,28 @@
   <si>
     <t>La fonction doit recevoir les données API depuis le paramètre pour ensuite les afficher.</t>
   </si>
+  <si>
+    <t>La fonction doit ajouter le produit choisi et les inputs à l'intérieur du tableau.array.
+Ensuite il doit envoyer les données à la page suivante avec la méthode POST. La fonction doit retourner le 
+local storage depuis le paramètre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La valeur retournée pourrait être erronée (un autre produit au lieu du produit choisit) ou l'affichage ne fonctionnerait pas.
+</t>
+  </si>
+  <si>
+    <t>La valeur retournée pourrait ne pas être disponible .</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -288,24 +283,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -529,79 +521,79 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="55.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="39.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="44.33203125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:26" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="43" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
@@ -609,19 +601,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -635,13 +627,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -655,13 +647,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -669,19 +661,19 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>40</v>
+      <c r="F6" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -689,19 +681,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -709,79 +701,79 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -5721,5 +5713,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>